<commit_message>
Saving results of netfit prediction
</commit_message>
<xml_diff>
--- a/Results/Predictive Modeling/Model comparison.xlsx
+++ b/Results/Predictive Modeling/Model comparison.xlsx
@@ -399,7 +399,7 @@
   <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -445,6 +445,15 @@
       <c r="D3">
         <v>0.97936509999999999</v>
       </c>
+      <c r="E3">
+        <v>0.98809519999999995</v>
+      </c>
+      <c r="F3">
+        <v>0.91666669999999995</v>
+      </c>
+      <c r="G3">
+        <v>0.96031750000000005</v>
+      </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">

</xml_diff>

<commit_message>
Updated Analysis, added some clustering with predictors
</commit_message>
<xml_diff>
--- a/Results/Predictive Modeling/Model comparison.xlsx
+++ b/Results/Predictive Modeling/Model comparison.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="10">
   <si>
     <t>Training</t>
   </si>
@@ -45,6 +45,15 @@
   </si>
   <si>
     <t xml:space="preserve"> ROC </t>
+  </si>
+  <si>
+    <t>SVM C = 1</t>
+  </si>
+  <si>
+    <t>Alpha = 0.75</t>
+  </si>
+  <si>
+    <t>Lambda = 0.25</t>
   </si>
 </sst>
 </file>
@@ -399,7 +408,7 @@
   <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -437,13 +446,13 @@
         <v>0</v>
       </c>
       <c r="B3">
-        <v>0.99206349999999999</v>
+        <v>0.98095239999999995</v>
       </c>
       <c r="C3">
-        <v>0.73333329999999997</v>
+        <v>0.63333329999999999</v>
       </c>
       <c r="D3">
-        <v>0.97936509999999999</v>
+        <v>1</v>
       </c>
       <c r="E3">
         <v>0.98809519999999995</v>
@@ -458,6 +467,28 @@
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>0.911111</v>
+      </c>
+      <c r="G4">
+        <v>0.99047620000000003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
-Updated table: compare glmnet vs svm    - added test errors - modified a few lines in predictivemodelingVY.rmd
</commit_message>
<xml_diff>
--- a/Results/Predictive Modeling/Model comparison.xlsx
+++ b/Results/Predictive Modeling/Model comparison.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>Training</t>
   </si>
@@ -44,9 +44,6 @@
     <t>Spec</t>
   </si>
   <si>
-    <t xml:space="preserve"> ROC </t>
-  </si>
-  <si>
     <t>SVM C = 1</t>
   </si>
   <si>
@@ -54,6 +51,15 @@
   </si>
   <si>
     <t>Lambda = 0.25</t>
+  </si>
+  <si>
+    <t>AUC</t>
+  </si>
+  <si>
+    <t>0.977+-0.024</t>
+  </si>
+  <si>
+    <t>0.978+-0.05</t>
   </si>
 </sst>
 </file>
@@ -405,15 +411,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N12"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>2</v>
       </c>
@@ -421,9 +427,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -432,7 +438,7 @@
         <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F2" t="s">
         <v>4</v>
@@ -441,7 +447,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -464,60 +470,28 @@
         <v>0.96031750000000005</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4">
-        <v>0.911111</v>
-      </c>
-      <c r="G4">
-        <v>0.99047620000000003</v>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
         <v>8</v>
-      </c>
-      <c r="E6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="K9" t="s">
-        <v>0</v>
-      </c>
-      <c r="L9" t="s">
-        <v>1</v>
-      </c>
-      <c r="M9" t="s">
-        <v>0</v>
-      </c>
-      <c r="N9" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="J10" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="J11" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="J12" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Put all of the statistical analysis images and write up for the poster into 'poster/statistical analysis' subdirectory
</commit_message>
<xml_diff>
--- a/Results/Predictive Modeling/Model comparison.xlsx
+++ b/Results/Predictive Modeling/Model comparison.xlsx
@@ -75,15 +75,33 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -91,12 +109,135 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -414,72 +555,86 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection sqref="A1:G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="13.21875" customWidth="1"/>
+    <col min="5" max="5" width="11.5546875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B1" t="s">
+      <c r="A1" s="12"/>
+      <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="C1" s="3"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="7" t="s">
         <v>3</v>
       </c>
+      <c r="F1" s="8"/>
+      <c r="G1" s="9"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B2" t="s">
+      <c r="A2" s="13"/>
+      <c r="B2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="6">
         <v>0.98095239999999995</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="6">
         <v>0.63333329999999999</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="6">
         <v>1</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="11">
         <v>0.98809519999999995</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="11">
         <v>0.91666669999999995</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="11">
         <v>0.96031750000000005</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E4" t="s">
+      <c r="C4" s="14"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="11" t="s">
         <v>11</v>
       </c>
+      <c r="F4" s="16"/>
+      <c r="G4" s="17"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
@@ -495,6 +650,13 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="F4:G4"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>